<commit_message>
updated code & added some new folders
</commit_message>
<xml_diff>
--- a/processed_data/Trial_CalCOFI_Report_Data_R_format_2-2025.xlsx
+++ b/processed_data/Trial_CalCOFI_Report_Data_R_format_2-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanasevigny/git/ENSO_CalCOFI_dispersals2024/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BC5B40-DCA0-9145-B984-A30C515C0D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DBAF3D-BCD2-6748-A47D-47550438586C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34180" yWindow="1220" windowWidth="26440" windowHeight="15440" xr2:uid="{CACEE650-D14E-3646-B9DB-ADC0E7588080}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t>Report_Volume</t>
   </si>
@@ -540,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBA690B-CDCD-A845-A10E-624E0246FAD3}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -858,14 +858,10 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3">
-        <v>21094</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
@@ -885,257 +881,102 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3">
-        <v>21276</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="2">
-        <v>32.713002000000003</v>
-      </c>
-      <c r="G13" s="2">
-        <v>-117.25765199999999</v>
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="4">
+        <v>28</v>
+      </c>
+      <c r="G13" s="4">
+        <v>-114.27384000000001</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3">
-        <v>15067</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="4">
-        <v>28</v>
-      </c>
-      <c r="G14" s="4">
-        <v>-114.27384000000001</v>
+        <v>17</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2">
+        <v>34.448242</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-120.472067</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3">
-        <v>21155</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>9</v>
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="4">
-        <v>28</v>
-      </c>
-      <c r="G15" s="4">
-        <v>-114.27384000000001</v>
+        <v>20</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2">
+        <v>34.448242</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-120.472067</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3">
-        <v>21155</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="2">
-        <v>34.448242</v>
-      </c>
-      <c r="G16" s="2">
-        <v>-120.472067</v>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="4">
+        <v>30.963701</v>
+      </c>
+      <c r="G16" s="4">
+        <v>-116.334789</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>9</v>
-      </c>
-      <c r="B17" s="3">
-        <v>21276</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="2">
-        <v>34.448242</v>
-      </c>
-      <c r="G17" s="2">
-        <v>-120.472067</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>9</v>
-      </c>
-      <c r="B18" s="3">
-        <v>21520</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="4">
-        <v>28</v>
-      </c>
-      <c r="G18" s="4">
-        <v>-114.27384000000001</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>11</v>
-      </c>
-      <c r="B19" s="5">
-        <v>21885</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="4">
-        <v>28</v>
-      </c>
-      <c r="G19" s="4">
-        <v>-114.27384000000001</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>22</v>
-      </c>
-      <c r="B20" s="5">
-        <v>28491</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="4">
-        <v>30.963701</v>
-      </c>
-      <c r="G20" s="4">
-        <v>-116.334789</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5">
-        <v>25204</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="2">
-        <v>32.713002000000003</v>
-      </c>
-      <c r="G21" s="2">
-        <v>-117.25765199999999</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" s="2"/>
+      <c r="I16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>